<commit_message>
Added currency db feature
</commit_message>
<xml_diff>
--- a/Microservices/fundhandling/src/main/java/com/mutualfundtrading/fundhandling/upload/funds.xlsx
+++ b/Microservices/fundhandling/src/main/java/com/mutualfundtrading/fundhandling/upload/funds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krigudip\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somchakr\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Goldman</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Axis Bank</t>
+  </si>
+  <si>
+    <t>T+2</t>
+  </si>
+  <si>
+    <t>T+3</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,8 +479,8 @@
       <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>26</v>
       </c>
       <c r="E3">
         <v>25.6</v>
@@ -499,8 +505,8 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" t="s">
+        <v>26</v>
       </c>
       <c r="E4">
         <v>12.1</v>
@@ -525,8 +531,8 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
-        <v>2</v>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2.5</v>
@@ -551,8 +557,8 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
       <c r="E6">
         <v>3.5</v>
@@ -577,8 +583,8 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>2</v>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
       <c r="E7">
         <v>400</v>
@@ -603,8 +609,8 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>3</v>
+      <c r="D8" t="s">
+        <v>26</v>
       </c>
       <c r="E8">
         <v>6.5</v>
@@ -629,8 +635,8 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9">
-        <v>2</v>
+      <c r="D9" t="s">
+        <v>27</v>
       </c>
       <c r="E9">
         <v>233.5</v>

</xml_diff>